<commit_message>
Breakout Prompts to external text files.
</commit_message>
<xml_diff>
--- a/Zephyr_Test_Cases_Output.xlsx
+++ b/Zephyr_Test_Cases_Output.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +538,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify date range filtering functionality</t>
+          <t>Verify amount filter and sort functionality</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -547,13 +546,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click the filter icon on the Date column</t>
+          <t>Apply amount filter for transactions greater than $1000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Date filter options are displayed</t>
+          <t>Only transactions with amounts exceeding $1000 are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -568,8 +567,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is logged in and on transaction list view with multiple records present
-Transaction list shows filtered date range results</t>
+          <t>User is on the transaction list page with 100 transactions loaded
+Transaction list shows filtered and sorted results</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -637,7 +636,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify date range filtering functionality</t>
+          <t>Verify amount filter and sort functionality</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -645,13 +644,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Set date range from 2024-01-01 to 2024-01-31</t>
+          <t>Sort the filtered results by date in descending order</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Date range is applied</t>
+          <t>Transactions are arranged from newest to oldest date while maintaining the amount filter</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -666,8 +665,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is logged in and on transaction list view with multiple records present
-Transaction list shows filtered date range results</t>
+          <t>User is on the transaction list page with 100 transactions loaded
+Transaction list shows filtered and sorted results</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -724,202 +723,6 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verify date range filtering functionality</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Verify displayed transactions</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Only transactions between 2024-01-01 and 2024-01-31 are shown</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>User is logged in and on transaction list view with multiple records present
-Transaction list shows filtered date range results</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Verify date range filtering functionality</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Check filter icon state</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Filter icon displays in active state</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>User is logged in and on transaction list view with multiple records present
-Transaction list shows filtered date range results</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S5" t="n">
-        <v>37</v>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1057,7 +860,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify sorting of filtered transactions</t>
+          <t>Verify filter clearing on Copilot refresh</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1065,13 +868,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click sort icon on Date column</t>
+          <t>Trigger Copilot to return new transaction data</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sort options are displayed</t>
+          <t>Date filter is automatically cleared</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1086,8 +889,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User has filtered transactions to show amounts greater than $1000
-Filtered transactions remain sorted by date</t>
+          <t>User is on the transaction list page with date filter applied for last 30 days
+Transaction list shows unfiltered new data</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1155,7 +958,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify sorting of filtered transactions</t>
+          <t>Verify filter clearing on Copilot refresh</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1163,13 +966,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Verify sorted transactions</t>
+          <t>Observe the transaction list</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Transactions are sorted by date while maintaining $1000+ filter</t>
+          <t>All new transaction data is displayed without any filters applied</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1184,8 +987,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User has filtered transactions to show amounts greater than $1000
-Filtered transactions remain sorted by date</t>
+          <t>User is on the transaction list page with date filter applied for last 30 days
+Transaction list shows unfiltered new data</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1258,7 +1061,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1379,7 +1182,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify multiple column filter functionality</t>
+          <t>Verify sort persistence with filtered results</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1387,13 +1190,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply Amount filter for values above $500</t>
+          <t>Apply filter for transaction type 'Credit'</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Only transactions above $500 are displayed</t>
+          <t>Only credit transactions are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1408,8 +1211,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on transaction list view
-Multiple filters are successfully applied</t>
+          <t>User is on the transaction list page with transactions sorted by amount in ascending order
+Transaction list shows filtered credit transactions in sorted order</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1477,7 +1280,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify multiple column filter functionality</t>
+          <t>Verify sort persistence with filtered results</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1485,13 +1288,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Apply Transaction Type filter for Wire Transfers</t>
+          <t>Verify sort order</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Only wire transfers above $500 are displayed</t>
+          <t>Credit transactions remain sorted by amount in ascending order</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1506,8 +1309,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is on transaction list view
-Multiple filters are successfully applied</t>
+          <t>User is on the transaction list page with transactions sorted by amount in ascending order
+Transaction list shows filtered credit transactions in sorted order</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1564,104 +1367,6 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verify multiple column filter functionality</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Verify filter icons</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Both column filters show active state</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>User is on transaction list view
-Multiple filters are successfully applied</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1678,7 +1383,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1799,7 +1504,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify clear all filters functionality</t>
+          <t>Verify multiple column filtering</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1807,13 +1512,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click Clear All Filters button</t>
+          <t>Apply date filter for last 7 days</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>All filters are removed</t>
+          <t>Only transactions from the last 7 days are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1828,8 +1533,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Multiple filters are active on transaction list
-Transaction list returns to unfiltered state</t>
+          <t>User is on the transaction list page
+Transaction list shows results matching both filter criteria</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1897,7 +1602,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify clear all filters functionality</t>
+          <t>Verify multiple column filtering</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1905,13 +1610,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Verify transaction list</t>
+          <t>Apply amount filter for greater than $500</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Complete unfiltered transaction list is displayed</t>
+          <t>Only transactions meeting both criteria are displayed: last 7 days AND amount &gt; $500</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1926,8 +1631,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Multiple filters are active on transaction list
-Transaction list returns to unfiltered state</t>
+          <t>User is on the transaction list page
+Transaction list shows results matching both filter criteria</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1984,104 +1689,6 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verify clear all filters functionality</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Check filter icons</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>No filter icons show active state</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Multiple filters are active on transaction list
-Transaction list returns to unfiltered state</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -2098,7 +1705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2219,7 +1826,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify empty filter results handling</t>
+          <t>Verify help guide filtering documentation</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -2227,13 +1834,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply Transaction Type filter for Check</t>
+          <t>Open the help guide</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Filter is applied</t>
+          <t>Help guide is displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -2248,8 +1855,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on transaction list view
-System properly handles no matching results</t>
+          <t>User has access to the help guide
+User can access comprehensive filtering documentation</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -2317,7 +1924,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify empty filter results handling</t>
+          <t>Verify help guide filtering documentation</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -2325,13 +1932,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Verify empty results message</t>
+          <t>Navigate to filtering section</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>'No matching transactions found' message is displayed</t>
+          <t>Filtering documentation is visible with examples for each filter type</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -2346,8 +1953,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is on transaction list view
-System properly handles no matching results</t>
+          <t>User has access to the help guide
+User can access comprehensive filtering documentation</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -2404,622 +2011,6 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verify empty filter results handling</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Verify clear filter option</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Option to clear filters is visible and clickable</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>User is on transaction list view
-System properly handles no matching results</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>External id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Test Summary</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Step</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Test Data</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Assigned To</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>jira-customfield-checkbox</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Epic Link</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Linked issues</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Labels</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Issue Key [To add steps]</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Issue Link Type</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Issues Key To Link</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Sprint</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Cascade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Verify filter persistence across page navigation</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Navigate away from transaction list page</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>User leaves transaction list view</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Filters are applied to transaction list
-Filters persist through page navigation</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>37</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Verify filter persistence across page navigation</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Return to transaction list page</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Transaction list page loads</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Filters are applied to transaction list
-Filters persist through page navigation</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
-        <v>37</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verify filter persistence across page navigation</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Verify filter state</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Previously applied filters are still active</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Filters are applied to transaction list
-Filters persist through page navigation</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Verify filter persistence across page navigation</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Verify filtered results</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Filtered results are displayed as before navigation</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Filters are applied to transaction list
-Filters persist through page navigation</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S5" t="n">
-        <v>37</v>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>

</xml_diff>

<commit_message>
Set up additional external rules files.
</commit_message>
<xml_diff>
--- a/Zephyr_Test_Cases_Output.xlsx
+++ b/Zephyr_Test_Cases_Output.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,7 +537,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify amount filter and sort functionality</t>
+          <t>Verify single amount filter functionality</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -546,13 +545,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply amount filter for transactions greater than $1000</t>
+          <t>Click on amount filter option</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Only transactions with amounts exceeding $1000 are displayed</t>
+          <t>Amount filter dropdown is displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -567,8 +566,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on the transaction list page with 100 transactions loaded
-Transaction list shows filtered and sorted results</t>
+          <t>User is logged in as investigator and on transaction list page
+Amount filter is successfully applied</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -636,7 +635,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify amount filter and sort functionality</t>
+          <t>Verify single amount filter functionality</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -644,13 +643,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sort the filtered results by date in descending order</t>
+          <t>Select 'Greater than $1000' option</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Transactions are arranged from newest to oldest date while maintaining the amount filter</t>
+          <t>Only transactions over $1000 are shown in the list</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -665,8 +664,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is on the transaction list page with 100 transactions loaded
-Transaction list shows filtered and sorted results</t>
+          <t>User is logged in as investigator and on transaction list page
+Amount filter is successfully applied</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -723,6 +722,202 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Verify single amount filter functionality</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Check transaction count</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Count reflects number of filtered transactions</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is logged in as investigator and on transaction list page
+Amount filter is successfully applied</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>GenAI_Test_Case</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Verify single amount filter functionality</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Verify filter indicator</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Filter indicator is visible in the UI</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>User is logged in as investigator and on transaction list page
+Amount filter is successfully applied</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>GenAI_Test_Case</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>37</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -739,7 +934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -860,7 +1055,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify filter clearing on Copilot refresh</t>
+          <t>Verify multiple concurrent filters functionality</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -868,13 +1063,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Trigger Copilot to return new transaction data</t>
+          <t>Apply amount filter for 'Greater than $500'</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Date filter is automatically cleared</t>
+          <t>Transactions over $500 are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -889,8 +1084,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on the transaction list page with date filter applied for last 30 days
-Transaction list shows unfiltered new data</t>
+          <t>User is logged in as investigator and on transaction list page
+Multiple filters are successfully applied</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -958,7 +1153,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify filter clearing on Copilot refresh</t>
+          <t>Verify multiple concurrent filters functionality</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -966,13 +1161,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Observe the transaction list</t>
+          <t>Apply date filter for 'Last 7 days'</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>All new transaction data is displayed without any filters applied</t>
+          <t>Only transactions matching both amount and date criteria are shown</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -987,8 +1182,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is on the transaction list page with date filter applied for last 30 days
-Transaction list shows unfiltered new data</t>
+          <t>User is logged in as investigator and on transaction list page
+Multiple filters are successfully applied</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1045,6 +1240,104 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Verify multiple concurrent filters functionality</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Check filter indicators</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Two separate filter indicators are visible in the UI</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is logged in as investigator and on transaction list page
+Multiple filters are successfully applied</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>GenAI_Test_Case</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1182,7 +1475,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify sort persistence with filtered results</t>
+          <t>Verify filter persistence across navigation</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1190,13 +1483,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply filter for transaction type 'Credit'</t>
+          <t>Navigate to a different page</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Only credit transactions are displayed</t>
+          <t>Page navigation is successful</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1211,8 +1504,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on the transaction list page with transactions sorted by amount in ascending order
-Transaction list shows filtered credit transactions in sorted order</t>
+          <t>User has applied filters to transaction list
+Filter settings are preserved across navigation</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1280,7 +1573,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify sort persistence with filtered results</t>
+          <t>Verify filter persistence across navigation</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1288,13 +1581,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Verify sort order</t>
+          <t>Return to transaction list page</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Credit transactions remain sorted by amount in ascending order</t>
+          <t>Previously applied filters remain active and results are filtered accordingly</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1309,8 +1602,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is on the transaction list page with transactions sorted by amount in ascending order
-Transaction list shows filtered credit transactions in sorted order</t>
+          <t>User has applied filters to transaction list
+Filter settings are preserved across navigation</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1504,7 +1797,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify multiple column filtering</t>
+          <t>Verify empty results handling</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1512,13 +1805,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply date filter for last 7 days</t>
+          <t>Apply filters that result in no matching transactions</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Only transactions from the last 7 days are displayed</t>
+          <t>'No matching transactions' message is displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1533,8 +1826,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on the transaction list page
-Transaction list shows results matching both filter criteria</t>
+          <t>User is on transaction list page
+Empty state handling is properly displayed</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1602,7 +1895,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify multiple column filtering</t>
+          <t>Verify empty results handling</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1610,13 +1903,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Apply amount filter for greater than $500</t>
+          <t>Verify clear filters option</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Only transactions meeting both criteria are displayed: last 7 days AND amount &gt; $500</t>
+          <t>Option to clear filters is visible and clickable</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1631,330 +1924,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is on the transaction list page
-Transaction list shows results matching both filter criteria</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
-        <v>37</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>External id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Test Summary</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Step</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Test Data</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Assigned To</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>jira-customfield-checkbox</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Epic Link</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Linked issues</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Labels</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Issue Key [To add steps]</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Issue Link Type</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Issues Key To Link</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Sprint</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Cascade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Verify help guide filtering documentation</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Open the help guide</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Help guide is displayed</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>User has access to the help guide
-User can access comprehensive filtering documentation</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>37</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Verify help guide filtering documentation</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Navigate to filtering section</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Filtering documentation is visible with examples for each filter type</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>User has access to the help guide
-User can access comprehensive filtering documentation</t>
+          <t>User is on transaction list page
+Empty state handling is properly displayed</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>

<commit_message>
Change Temp of LLM Model
</commit_message>
<xml_diff>
--- a/Zephyr_Test_Cases_Output.xlsx
+++ b/Zephyr_Test_Cases_Output.xlsx
@@ -11,6 +11,8 @@
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,7 +539,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify single amount filter functionality</t>
+          <t>Verify single date filter functionality</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -545,13 +547,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click on amount filter option</t>
+          <t>Click on date filter dropdown</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Amount filter dropdown is displayed</t>
+          <t>Date filter options are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -567,7 +569,7 @@
       <c r="I2" t="inlineStr">
         <is>
           <t>User is logged in as investigator and on transaction list page
-Amount filter is successfully applied</t>
+Date filter is applied showing last 7 days of transactions</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -635,7 +637,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify single amount filter functionality</t>
+          <t>Verify single date filter functionality</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -643,13 +645,15 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Select 'Greater than $1000' option</t>
+          <t>Select 'Last 7 days' option</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Only transactions over $1000 are shown in the list</t>
+          <t>1. Only transactions from last 7 days are shown
+2. Date filter indicator shows as active
+3. Transaction count updates to show filtered total</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -665,7 +669,7 @@
       <c r="I3" t="inlineStr">
         <is>
           <t>User is logged in as investigator and on transaction list page
-Amount filter is successfully applied</t>
+Date filter is applied showing last 7 days of transactions</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -722,202 +726,6 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verify single amount filter functionality</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Check transaction count</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Count reflects number of filtered transactions</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>User is logged in as investigator and on transaction list page
-Amount filter is successfully applied</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Verify single amount filter functionality</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Verify filter indicator</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Filter indicator is visible in the UI</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>User is logged in as investigator and on transaction list page
-Amount filter is successfully applied</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S5" t="n">
-        <v>37</v>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -934,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1055,7 +863,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify multiple concurrent filters functionality</t>
+          <t>Verify multiple filter combination</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1063,13 +871,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply amount filter for 'Greater than $500'</t>
+          <t>Apply amount filter for 'Greater than $1000'</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Transactions over $500 are displayed</t>
+          <t>1. Only transactions matching both date and amount criteria are displayed
+2. Both filter indicators show as active
+3. Transaction count updates to reflect combined filters</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1084,8 +894,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is logged in as investigator and on transaction list page
-Multiple filters are successfully applied</t>
+          <t>User has date filter for 'Last 7 days' already applied
+Multiple filters are applied showing filtered transaction subset</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1142,202 +952,6 @@
         </is>
       </c>
       <c r="U2" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Verify multiple concurrent filters functionality</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Apply date filter for 'Last 7 days'</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Only transactions matching both amount and date criteria are shown</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>User is logged in as investigator and on transaction list page
-Multiple filters are successfully applied</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
-        <v>37</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Verify multiple concurrent filters functionality</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Check filter indicators</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Two separate filter indicators are visible in the UI</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>User is logged in as investigator and on transaction list page
-Multiple filters are successfully applied</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1354,7 +968,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1475,7 +1089,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify filter persistence across navigation</t>
+          <t>Verify individual filter removal</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1483,13 +1097,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Navigate to a different page</t>
+          <t>Click to clear date filter</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Page navigation is successful</t>
+          <t>1. Date filter is removed
+2. Other active filters remain unchanged
+3. Results update to show transactions matching remaining filters</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1504,8 +1120,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User has applied filters to transaction list
-Filter settings are preserved across navigation</t>
+          <t>Multiple filters are active on transaction list
+Selected filter is removed while others remain active</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1562,104 +1178,6 @@
         </is>
       </c>
       <c r="U2" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Verify filter persistence across navigation</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Return to transaction list page</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Previously applied filters remain active and results are filtered accordingly</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>User has applied filters to transaction list
-Filter settings are preserved across navigation</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
-        <v>37</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1676,7 +1194,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1797,7 +1315,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify empty results handling</t>
+          <t>Verify sorting of filtered results</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1805,13 +1323,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply filters that result in no matching transactions</t>
+          <t>Click amount column header</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>'No matching transactions' message is displayed</t>
+          <t>1. Filtered credit transactions are sorted by amount
+2. Only credit transactions remain visible in sorted order</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1826,8 +1345,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on transaction list page
-Empty state handling is properly displayed</t>
+          <t>Transaction Type filter for 'Credit' is applied
+Filtered results are sorted by selected column</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1889,99 +1408,451 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>4</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Verify empty results handling</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Verify clear filters option</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Option to clear filters is visible and clickable</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>External id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Test Summary</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>OrderId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Step</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Test Data</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Expected Result</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Assigned To</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>jira-customfield-checkbox</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Epic Link</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Linked issues</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Labels</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Issue Key [To add steps]</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Issue Link Type</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Issues Key To Link</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Sprint</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Cascade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Verify Copilot command filter clearing</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Execute Copilot command that returns transaction results</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1. All existing filters are cleared
+2. New Copilot results are displayed without filters</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>6414a0cd67102fc717c034d7</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Active filters are applied to transaction list
+Copilot results displayed with no active filters</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>GenAI_Test_Case</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>37</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>External id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Test Summary</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>OrderId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Step</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Test Data</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Expected Result</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Assigned To</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>jira-customfield-checkbox</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Epic Link</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Linked issues</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Labels</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Issue Key [To add steps]</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Issue Link Type</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Issues Key To Link</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Sprint</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Cascade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Verify no matching results handling</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Apply filters that result in no matching transactions</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1. 'No matching transactions found' message is displayed
+2. Option to clear all filters is shown</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>User is on transaction list page
-Empty state handling is properly displayed</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
+System shows appropriate messaging for no results</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Core</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>external</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>INVHUB-10821</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>blocks</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>GenAI_Test_Case</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>IM-5000</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>blocks</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>IM-3000</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>3 - Medium</t>
         </is>
       </c>
-      <c r="S3" t="n">
+      <c r="S2" t="n">
         <v>37</v>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>Release-1.0</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>

</xml_diff>

<commit_message>
Updated docs and Zephyr Import
</commit_message>
<xml_diff>
--- a/Zephyr_Test_Cases_Output.xlsx
+++ b/Zephyr_Test_Cases_Output.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +538,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify single date filter functionality</t>
+          <t>Verify filtering transactions by Base Amount</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -547,13 +546,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click on date filter dropdown</t>
+          <t>Navigate to the transaction list screen</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Date filter options are displayed</t>
+          <t>Transaction list screen is displayed with all transactions</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -568,8 +567,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is logged in as investigator and on transaction list page
-Date filter is applied showing last 7 days of transactions</t>
+          <t>User is logged into the application and has access to the transaction list screen with multiple transactions
+Applied filter is shown above the transaction list table</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -594,7 +593,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>GenAI_Test_Case</t>
+          <t>AINative(GenAI_Test_Case)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -637,7 +636,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify single date filter functionality</t>
+          <t>Verify filtering transactions by Base Amount</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -645,15 +644,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Select 'Last 7 days' option</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Click the filter button for Base Amount column</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Base Amount column</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1. Only transactions from last 7 days are shown
-2. Date filter indicator shows as active
-3. Transaction count updates to show filtered total</t>
+          <t>Filter options for Base Amount are displayed</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -668,8 +669,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is logged in as investigator and on transaction list page
-Date filter is applied showing last 7 days of transactions</t>
+          <t>User is logged into the application and has access to the transaction list screen with multiple transactions
+Applied filter is shown above the transaction list table</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -694,7 +695,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>GenAI_Test_Case</t>
+          <t>AINative(GenAI_Test_Case)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -726,6 +727,210 @@
         </is>
       </c>
       <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Verify filtering transactions by Base Amount</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Select the most frequent amount value in the column</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Most frequent Base Amount: $1000.00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Most frequent amount value is selected</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is logged into the application and has access to the transaction list screen with multiple transactions
+Applied filter is shown above the transaction list table</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Verify filtering transactions by Base Amount</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Verify filter button appearance and filtered results</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$1000.00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Filter button icon changes from hollow to filled, only transactions with selected amount are displayed</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>User is logged into the application and has access to the transaction list screen with multiple transactions
+Applied filter is shown above the transaction list table</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>37</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -742,7 +947,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -863,7 +1068,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify multiple filter combination</t>
+          <t>Verify filtering transactions by date range</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -871,15 +1076,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply amount filter for 'Greater than $1000'</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Click the filter button for Transaction Date column</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Transaction Date column</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1. Only transactions matching both date and amount criteria are displayed
-2. Both filter indicators show as active
-3. Transaction count updates to reflect combined filters</t>
+          <t>Date range filter options are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -894,8 +1101,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User has date filter for 'Last 7 days' already applied
-Multiple filters are applied showing filtered transaction subset</t>
+          <t>User is on the transaction list screen with transactions from multiple dates
+Transaction list shows only transactions within selected date range</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -920,7 +1127,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>GenAI_Test_Case</t>
+          <t>AINative(GenAI_Test_Case)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -952,6 +1159,312 @@
         </is>
       </c>
       <c r="U2" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Verify filtering transactions by date range</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Enter the oldest date in the from field</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Oldest date is entered in from field</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with transactions from multiple dates
+Transaction list shows only transactions within selected date range</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>37</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Verify filtering transactions by date range</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Enter the second oldest date in the to field</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2023-01-15</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Second oldest date is entered in to field</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with transactions from multiple dates
+Transaction list shows only transactions within selected date range</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Verify filtering transactions by date range</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Verify filtered results</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Date range: 2023-01-01 to 2023-01-15</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Only transactions within specified date range are displayed</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with transactions from multiple dates
+Transaction list shows only transactions within selected date range</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>37</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -968,7 +1481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1089,7 +1602,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify individual filter removal</t>
+          <t>Verify multiple filters and sorting functionality</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1097,15 +1610,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click to clear date filter</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Filter Transaction Type column for CASH</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Transaction Type: CASH</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1. Date filter is removed
-2. Other active filters remain unchanged
-3. Results update to show transactions matching remaining filters</t>
+          <t>Only CASH transactions are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1120,8 +1635,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Multiple filters are active on transaction list
-Selected filter is removed while others remain active</t>
+          <t>User is on the transaction list screen with multiple transaction types and accounts
+Filtered transactions remain sorted by amount</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1146,7 +1661,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>GenAI_Test_Case</t>
+          <t>AINative(GenAI_Test_Case)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1178,6 +1693,206 @@
         </is>
       </c>
       <c r="U2" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Verify multiple filters and sorting functionality</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Filter Account ID column for ACC001</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Account ID: ACC001</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Only CASH transactions for ACC001 are displayed</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with multiple transaction types and accounts
+Filtered transactions remain sorted by amount</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>37</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Verify multiple filters and sorting functionality</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sort the Base Amount column</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Filtered transactions are sorted by amount while maintaining filters</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with multiple transaction types and accounts
+Filtered transactions remain sorted by amount</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1194,7 +1909,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1315,7 +2030,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify sorting of filtered results</t>
+          <t>Verify clearing all filters functionality</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1323,14 +2038,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click amount column header</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Filter Debit/Credit column for Debit</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Transaction Type: Debit</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1. Filtered credit transactions are sorted by amount
-2. Only credit transactions remain visible in sorted order</t>
+          <t>Only Debit transactions are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1345,8 +2063,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Transaction Type filter for 'Credit' is applied
-Filtered results are sorted by selected column</t>
+          <t>User is on the transaction list screen with multiple filters applied
+All filters are cleared and complete transaction list is displayed</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1371,7 +2089,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>GenAI_Test_Case</t>
+          <t>AINative(GenAI_Test_Case)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1403,6 +2121,206 @@
         </is>
       </c>
       <c r="U2" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Verify clearing all filters functionality</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Filter Transaction Type column for CASH</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Transaction Type: CASH</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Only Debit CASH transactions are displayed</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with multiple filters applied
+All filters are cleared and complete transaction list is displayed</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>37</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Verify clearing all filters functionality</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Click the Clear All Filters button</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>All transactions are displayed and no filter icons are filled</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with multiple filters applied
+All filters are cleared and complete transaction list is displayed</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1419,7 +2337,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1540,7 +2458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify Copilot command filter clearing</t>
+          <t>Verify filtering after ChatAI interaction</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1548,14 +2466,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Execute Copilot command that returns transaction results</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Request ChatAI to show transactions with most frequent Base Amount and CASH type</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Most frequent Base Amount: $1000.00, Type: CASH</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1. All existing filters are cleared
-2. New Copilot results are displayed without filters</t>
+          <t>ChatAI filters transactions as requested</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1570,8 +2491,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Active filters are applied to transaction list
-Copilot results displayed with no active filters</t>
+          <t>User is on the transaction list screen with ChatAI feature enabled
+Transactions are filtered by ChatAI criteria and Account ID</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1596,7 +2517,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>GenAI_Test_Case</t>
+          <t>AINative(GenAI_Test_Case)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -1633,226 +2554,201 @@
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>External id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Test Summary</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Step</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Test Data</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Assigned To</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>jira-customfield-checkbox</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Epic Link</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Linked issues</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Labels</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Issue Key [To add steps]</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Issue Link Type</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Issues Key To Link</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Sprint</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Cascade</t>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Verify filtering after ChatAI interaction</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Wait for transaction list refresh</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Transaction list updates with requested filters</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with ChatAI feature enabled
+Transactions are filtered by ChatAI criteria and Account ID</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>37</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Verify no matching results handling</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Apply filters that result in no matching transactions</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1. 'No matching transactions found' message is displayed
-2. Option to clear all filters is shown</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Verify filtering after ChatAI interaction</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Filter Account ID column for ACC001</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Account ID: ACC001</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Only ACC001 transactions are displayed while maintaining previous filters</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>6414a0cd67102fc717c034d7</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>User is on transaction list page
-System shows appropriate messaging for no results</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is on the transaction list screen with ChatAI feature enabled
+Transactions are filtered by ChatAI criteria and Account ID</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>Core</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>external</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>INVHUB-10821</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>GenAI_Test_Case</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>IM-5000</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>IM-3000</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>3 - Medium</t>
         </is>
       </c>
-      <c r="S2" t="n">
+      <c r="S4" t="n">
         <v>37</v>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>Release-1.0</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>

</xml_diff>

<commit_message>
Further Test Run - Feb12th
</commit_message>
<xml_diff>
--- a/Zephyr_Test_Cases_Output.xlsx
+++ b/Zephyr_Test_Cases_Output.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,13 +546,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Navigate to the transaction list page</t>
+          <t>Click on Transaction Date filter</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Transaction list page is displayed</t>
+          <t>Date filter options are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -568,7 +567,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is logged into the application and has access to the transaction list page
+          <t>User is on the Transaction List screen AND transaction list contains data
 Transaction list shows filtered results by date range</t>
         </is>
       </c>
@@ -645,13 +644,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Click on Transaction Date filter</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
+          <t>Enter from date in the filter</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2023-01-01</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Date filter options are displayed</t>
+          <t>From date is accepted</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -666,7 +669,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is logged into the application and has access to the transaction list page
+          <t>User is on the Transaction List screen AND transaction list contains data
 Transaction list shows filtered results by date range</t>
         </is>
       </c>
@@ -743,17 +746,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Enter the oldest date in the from field</t>
+          <t>Enter to date in the filter</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>From date is accepted</t>
+          <t>To date is accepted</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -768,7 +771,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>User is logged into the application and has access to the transaction list page
+          <t>User is on the Transaction List screen AND transaction list contains data
 Transaction list shows filtered results by date range</t>
         </is>
       </c>
@@ -845,17 +848,13 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Enter the second oldest date in the to field</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2023-01-31</t>
-        </is>
-      </c>
+          <t>Verify filter icon state</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>To date is accepted</t>
+          <t>Filter icon changes from hollow to filled</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -870,7 +869,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>User is logged into the application and has access to the transaction list page
+          <t>User is on the Transaction List screen AND transaction list contains data
 Transaction list shows filtered results by date range</t>
         </is>
       </c>
@@ -947,13 +946,13 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Verify filtered results</t>
+          <t>Check active filter display</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Only transactions within specified date range are displayed, filter icon is filled, and active filter appears above table</t>
+          <t>Active filter appears above transaction list table</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -968,7 +967,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>User is logged into the application and has access to the transaction list page
+          <t>User is on the Transaction List screen AND transaction list contains data
 Transaction list shows filtered results by date range</t>
         </is>
       </c>
@@ -1026,6 +1025,104 @@
         </is>
       </c>
       <c r="U6" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Filter transactions by date range</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Verify filtered results</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Only transactions between 2023-01-01 and 2023-01-15 are displayed</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by date range</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>37</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -1037,430 +1134,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>External id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Test Summary</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Step</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Test Data</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Assigned To</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>jira-customfield-checkbox</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Epic Link</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Linked issues</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Labels</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Issue Key [To add steps]</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Issue Link Type</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Issues Key To Link</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Sprint</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Cascade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Filter transactions by Base Amount</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Click on Base Amount filter</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Base Amount filter options are displayed</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>User is on the transaction list page
-Transaction list shows filtered results by amount</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>AINative(GenAI_Test_Case)</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>37</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Filter transactions by Base Amount</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Enter the most frequent amount value</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1000.00</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Amount value is accepted</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>User is on the transaction list page
-Transaction list shows filtered results by amount</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>AINative(GenAI_Test_Case)</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
-        <v>37</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Filter transactions by Base Amount</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Verify filtered results</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Only transactions with specified amount are displayed and filter icon is filled</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>User is on the transaction list page
-Transaction list shows filtered results by amount</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>AINative(GenAI_Test_Case)</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>37</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1583,11 +1256,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Apply and clear multiple filters</t>
+          <t>Filter transactions by Base Amount</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1595,17 +1268,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Apply Transaction Type filter</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CASH</t>
-        </is>
-      </c>
+          <t>Click on Base Amount filter</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CASH transactions are filtered</t>
+          <t>Base Amount filter options are displayed</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1620,8 +1289,530 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is on the transaction list page
-All filters are cleared and original transaction list is displayed</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by Base Amount</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S2" t="n">
+        <v>37</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Filter transactions by Base Amount</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Enter most frequent amount value</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Most frequent amount from Base Amount column</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Amount value is accepted</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by Base Amount</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S3" t="n">
+        <v>37</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Filter transactions by Base Amount</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Verify filtered results</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Only transactions with selected Base Amount are displayed</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by Base Amount</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>37</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Filter transactions by Base Amount</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Check filter icon state</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Filter icon changes from hollow to filled</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by Base Amount</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>37</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>External id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Test Summary</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>OrderId</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Step</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Test Data</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Expected Result</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Assigned To</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Comments</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Component</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>jira-customfield-checkbox</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Epic Link</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Linked issues</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Labels</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Issue Key [To add steps]</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Issue Link Type</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Issues Key To Link</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Sprint</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Version</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Cascade</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Apply and clear multiple filters</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Select Transaction Type filter</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Transaction Type filter options are displayed</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list returns to unfiltered state</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1697,17 +1888,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Apply Account ID filter</t>
+          <t>Select CASH from dropdown</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ACC123456</t>
+          <t>CASH</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Account ID transactions are filtered</t>
+          <t>CASH is selected as filter value</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1722,8 +1913,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is on the transaction list page
-All filters are cleared and original transaction list is displayed</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list returns to unfiltered state</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1799,13 +1990,13 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Verify Clear All Filters option</t>
+          <t>Select Account ID filter</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Clear All Filters option is visible</t>
+          <t>Account ID filter options are displayed</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -1820,8 +2011,8 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>User is on the transaction list page
-All filters are cleared and original transaction list is displayed</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list returns to unfiltered state</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1897,13 +2088,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Click Clear All Filters</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
+          <t>Enter Account ID</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ACC123456</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>All filter icons return to hollow state and no active filters appear</t>
+          <t>Account ID is accepted</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1918,8 +2113,8 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>User is on the transaction list page
-All filters are cleared and original transaction list is displayed</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list returns to unfiltered state</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1976,6 +2171,300 @@
         </is>
       </c>
       <c r="U5" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Apply and clear multiple filters</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Verify filter icons</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Both filter icons change from hollow to filled</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list returns to unfiltered state</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>37</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Apply and clear multiple filters</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Verify filtered results</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Only CASH transactions for ACC123456 are displayed</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list returns to unfiltered state</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>37</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Apply and clear multiple filters</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Click Clear All Filters button</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>All filters are removed and complete transaction list is displayed</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list returns to unfiltered state</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>37</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>
@@ -2113,7 +2602,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Sort filtered results</t>
+          <t>Sort filtered results by date</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -2121,13 +2610,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Click Account ID column header</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>Apply Base Amount filter</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Most frequent amount value</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Filtered results are sorted by Account ID</t>
+          <t>Base Amount filter is applied</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -2142,8 +2635,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Transaction list is filtered by DEBIT Transaction Type
-Filtered results are sorted while maintaining filter</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Filtered transactions are sorted by date</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -2211,7 +2704,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sort filtered results</t>
+          <t>Sort filtered results by date</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -2219,17 +2712,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Verify Transaction Type filter</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DEBIT</t>
-        </is>
-      </c>
+          <t>Click Transaction Date column header</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Transaction Type filter remains active</t>
+          <t>Transactions remain filtered by Base Amount and are sorted by Transaction Date</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -2244,8 +2733,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Transaction list is filtered by DEBIT Transaction Type
-Filtered results are sorted while maintaining filter</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Filtered transactions are sorted by date</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -2318,7 +2807,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2439,7 +2928,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Copilot interaction with filters</t>
+          <t>Filter after ChatAI interaction</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -2452,12 +2941,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Base Amount: 1000.00, Type: CASH</t>
+          <t>Base Amount = most frequent value, Type = CASH</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Existing filters are cleared</t>
+          <t>ChatAI filters transactions by most frequent Base Amount and CASH type</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -2472,8 +2961,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Transaction list is filtered by Base Amount
-Transaction list shows Copilot-filtered results</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by date range after ChatAI interaction</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -2541,7 +3030,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Copilot interaction with filters</t>
+          <t>Filter after ChatAI interaction</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -2549,13 +3038,13 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Verify transaction list update</t>
+          <t>Verify list refresh</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Transaction list updates with Copilot results</t>
+          <t>Transaction list refreshes with ChatAI filtered results</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -2570,334 +3059,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Transaction list is filtered by Base Amount
-Transaction list shows Copilot-filtered results</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>AINative(GenAI_Test_Case)</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S3" t="n">
-        <v>37</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>External id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Test Summary</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>OrderId</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Step</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Test Data</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Expected Result</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Assigned To</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Comments</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Component</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>jira-customfield-checkbox</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Epic Link</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Linked issues</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Labels</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Issue Key [To add steps]</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Issue Link Type</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Issues Key To Link</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Priority</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Sprint</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Cascade</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Apply filter after Copilot interaction</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Select Transaction Date filter</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Date filter options are displayed</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Copilot has displayed transaction results
-Copilot results are filtered by date range</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Core</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>external</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>INVHUB-10821</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>AINative(GenAI_Test_Case)</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>IM-5000</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>blocks</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>IM-3000</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>3 - Medium</t>
-        </is>
-      </c>
-      <c r="S2" t="n">
-        <v>37</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>Release-1.0</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>Dublin</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>6</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Apply filter after Copilot interaction</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Enter date range</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>From: 2023-01-01, To: 2023-01-31</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Date range is accepted</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>6414a0cd67102fc717c034d7</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Copilot has displayed transaction results
-Copilot results are filtered by date range</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by date range after ChatAI interaction</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -2961,11 +3124,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Apply filter after Copilot interaction</t>
+          <t>Filter after ChatAI interaction</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -2973,13 +3136,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Verify filtered results</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>Apply date range filter</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>From: 2023-01-01, To: 2023-01-15</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Transaction list updates with date-filtered results from Copilot's list</t>
+          <t>Date filter options are displayed</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -2994,8 +3161,8 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Copilot has displayed transaction results
-Copilot results are filtered by date range</t>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by date range after ChatAI interaction</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -3052,6 +3219,104 @@
         </is>
       </c>
       <c r="U4" t="inlineStr">
+        <is>
+          <t>Dublin</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Filter after ChatAI interaction</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Verify final filtered results</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Only transactions within date range are displayed and filter icon changes from hollow to filled</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>6414a0cd67102fc717c034d7</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>This test case has been built by GenAI Workbench for XL import via Internal Importer.</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>User is on the Transaction List screen AND transaction list contains data
+Transaction list shows filtered results by date range after ChatAI interaction</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>INVHUB-10821</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>AINative(GenAI_Test_Case)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>IM-5000</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>blocks</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>IM-3000</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>3 - Medium</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>37</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Release-1.0</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
         <is>
           <t>Dublin</t>
         </is>

</xml_diff>